<commit_message>
Correct data capture typo
</commit_message>
<xml_diff>
--- a/Data/UCT002 Cell Densities and Voltages.xlsx
+++ b/Data/UCT002 Cell Densities and Voltages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrence/GitHub/SISPS-EXP-PUB/SISPS-EXP-SOC/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CECADC-FED9-3748-80ED-10424E68B650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABE764E-2AB0-FC47-A1E7-0B319912367B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{C94DDB7A-C64A-7442-BB49-9D5A79F904E6}"/>
   </bookViews>
@@ -999,7 +999,7 @@
   <dimension ref="A1:F128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add Batch B Density Measurements taken by Lindo
</commit_message>
<xml_diff>
--- a/Data/UCT002 Cell Densities and Voltages.xlsx
+++ b/Data/UCT002 Cell Densities and Voltages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrence/GitHub/SISPS-EXP-PUB/SISPS-EXP-SOC/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4113F741-866D-5644-963C-EB5E0FB17A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741A0768-C6CE-C246-9FD3-2F888B1EFCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{C94DDB7A-C64A-7442-BB49-9D5A79F904E6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19780" xr2:uid="{C94DDB7A-C64A-7442-BB49-9D5A79F904E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="45">
   <si>
     <t>Hydrometer</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Baptured in the order of A10-A01, B10-B01 (lowest to highest concentration) with some exceptions.</t>
+  </si>
+  <si>
+    <t>Manually interpolated s.g. and T against standard data tables.</t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -585,6 +588,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -593,7 +641,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1"/>
@@ -661,6 +709,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent5" xfId="3" builtinId="46"/>
@@ -1001,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C591D5-9543-7B4E-8905-292C0A65DA99}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="143" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="143" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1012,7 +1063,7 @@
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="65" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
@@ -2054,9 +2105,15 @@
       <c r="C66" s="24">
         <v>2.16</v>
       </c>
-      <c r="D66" s="37"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="7"/>
+      <c r="D66" s="37">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="E66" s="10">
+        <v>21.8</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="13"/>
@@ -2166,9 +2223,16 @@
       <c r="C73" s="24">
         <v>2.1320000000000001</v>
       </c>
-      <c r="D73" s="37"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="7"/>
+      <c r="D73" s="37">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="E73" s="10">
+        <v>22</v>
+      </c>
+      <c r="F73" s="7" t="str">
+        <f>F66</f>
+        <v>Manually interpolated s.g. and T against standard data tables.</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="13"/>
@@ -2264,9 +2328,16 @@
       <c r="C79" s="24">
         <v>2.1080000000000001</v>
       </c>
-      <c r="D79" s="37"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="7"/>
+      <c r="D79" s="37">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="E79" s="10">
+        <v>22</v>
+      </c>
+      <c r="F79" s="7" t="str">
+        <f>F66</f>
+        <v>Manually interpolated s.g. and T against standard data tables.</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="13"/>
@@ -2390,8 +2461,16 @@
       <c r="C87" s="24">
         <v>2.0779999999999998</v>
       </c>
-      <c r="E87" s="10"/>
-      <c r="F87" s="7"/>
+      <c r="D87" s="37">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="E87" s="10">
+        <v>22.1</v>
+      </c>
+      <c r="F87" s="7" t="str">
+        <f>F66</f>
+        <v>Manually interpolated s.g. and T against standard data tables.</v>
+      </c>
     </row>
     <row r="88" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="16"/>
@@ -2485,9 +2564,16 @@
       <c r="C93" s="24">
         <v>2.06</v>
       </c>
-      <c r="D93" s="37"/>
-      <c r="E93" s="10"/>
-      <c r="F93" s="7"/>
+      <c r="D93" s="37">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="E93" s="10">
+        <v>22</v>
+      </c>
+      <c r="F93" s="7" t="str">
+        <f>F79</f>
+        <v>Manually interpolated s.g. and T against standard data tables.</v>
+      </c>
     </row>
     <row r="94" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="19"/>
@@ -2595,9 +2681,16 @@
       <c r="C100" s="27">
         <v>2.0419999999999998</v>
       </c>
-      <c r="D100" s="38"/>
-      <c r="E100" s="18"/>
-      <c r="F100" s="17"/>
+      <c r="D100" s="38">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="E100" s="18">
+        <v>22.2</v>
+      </c>
+      <c r="F100" s="22" t="str">
+        <f>F93</f>
+        <v>Manually interpolated s.g. and T against standard data tables.</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="32" t="s">
@@ -2609,9 +2702,16 @@
       <c r="C101" s="34">
         <v>2.0179999999999998</v>
       </c>
-      <c r="D101" s="39"/>
-      <c r="E101" s="9"/>
-      <c r="F101" s="35"/>
+      <c r="D101" s="39">
+        <v>0.245</v>
+      </c>
+      <c r="E101" s="9">
+        <v>22.2</v>
+      </c>
+      <c r="F101" s="43" t="str">
+        <f>F93</f>
+        <v>Manually interpolated s.g. and T against standard data tables.</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="13"/>
@@ -2627,7 +2727,7 @@
       <c r="E102" s="10">
         <v>22.7</v>
       </c>
-      <c r="F102" s="7"/>
+      <c r="F102" s="44"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="13"/>
@@ -2643,7 +2743,7 @@
       <c r="E103" s="10">
         <v>23</v>
       </c>
-      <c r="F103" s="7"/>
+      <c r="F103" s="44"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="13"/>
@@ -2659,7 +2759,7 @@
       <c r="E104" s="10">
         <v>22.9</v>
       </c>
-      <c r="F104" s="7"/>
+      <c r="F104" s="44"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="13"/>
@@ -2675,7 +2775,7 @@
       <c r="E105" s="10">
         <v>22.6</v>
       </c>
-      <c r="F105" s="7"/>
+      <c r="F105" s="44"/>
     </row>
     <row r="106" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="19"/>
@@ -2691,7 +2791,7 @@
       <c r="E106" s="21">
         <v>22.6</v>
       </c>
-      <c r="F106" s="22"/>
+      <c r="F106" s="45"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="12" t="s">
@@ -2703,9 +2803,16 @@
       <c r="C107" s="26">
         <v>2.0009999999999999</v>
       </c>
-      <c r="D107" s="36"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="6"/>
+      <c r="D107" s="36">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="E107" s="8">
+        <v>22.2</v>
+      </c>
+      <c r="F107" s="7" t="str">
+        <f>F101</f>
+        <v>Manually interpolated s.g. and T against standard data tables.</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="13"/>
@@ -2877,9 +2984,16 @@
       <c r="C118" s="25">
         <v>1.9490000000000001</v>
       </c>
-      <c r="D118" s="40"/>
-      <c r="E118" s="21"/>
-      <c r="F118" s="22"/>
+      <c r="D118" s="40">
+        <v>0.151</v>
+      </c>
+      <c r="E118" s="21">
+        <v>22.2</v>
+      </c>
+      <c r="F118" s="22" t="str">
+        <f>F107</f>
+        <v>Manually interpolated s.g. and T against standard data tables.</v>
+      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="12" t="s">
@@ -2891,9 +3005,16 @@
       <c r="C119" s="26">
         <v>1.9410000000000001</v>
       </c>
-      <c r="D119" s="36"/>
-      <c r="E119" s="8"/>
-      <c r="F119" s="6"/>
+      <c r="D119" s="36">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E119" s="8">
+        <v>22.2</v>
+      </c>
+      <c r="F119" s="43" t="str">
+        <f>F107</f>
+        <v>Manually interpolated s.g. and T against standard data tables.</v>
+      </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="13"/>
@@ -2909,7 +3030,7 @@
       <c r="E120" s="10">
         <v>22.8</v>
       </c>
-      <c r="F120" s="7"/>
+      <c r="F120" s="44"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="13"/>
@@ -2925,7 +3046,7 @@
       <c r="E121" s="10">
         <v>23.4</v>
       </c>
-      <c r="F121" s="7"/>
+      <c r="F121" s="44"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="13"/>
@@ -2941,7 +3062,7 @@
       <c r="E122" s="10">
         <v>22.6</v>
       </c>
-      <c r="F122" s="7"/>
+      <c r="F122" s="44"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="13"/>
@@ -2957,7 +3078,7 @@
       <c r="E123" s="10">
         <v>22.4</v>
       </c>
-      <c r="F123" s="7"/>
+      <c r="F123" s="44"/>
     </row>
     <row r="124" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A124" s="16"/>
@@ -2973,7 +3094,7 @@
       <c r="E124" s="18">
         <v>22.7</v>
       </c>
-      <c r="F124" s="17"/>
+      <c r="F124" s="45"/>
     </row>
     <row r="126" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
@@ -3001,6 +3122,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100006575BCBA265A4686164F43ED0EE98E" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc6516f22a5044b005c3cacc24834ea6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f7122e4b-9ebe-4e7f-8fe9-d038fef3055f" xmlns:ns3="760f229c-99bf-4186-a7de-2d3c0bf5f7b2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7008822f133d3a71b5c1cfc5b0ad87c8" ns2:_="" ns3:_="">
     <xsd:import namespace="f7122e4b-9ebe-4e7f-8fe9-d038fef3055f"/>
@@ -3249,16 +3379,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA47CC0C-1F10-407C-BD58-6EB010626F00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC9DE635-C370-4A82-BEF5-1F4956ED594C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3275,12 +3404,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA47CC0C-1F10-407C-BD58-6EB010626F00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>